<commit_message>
GDE-6716 - Addressed reviewpoints
- Updated correct screenshot path
- Removed comments
- Added pre and post processing
- Added BUS keyword in custom mapping
</commit_message>
<xml_diff>
--- a/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT03.xlsx
+++ b/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT03.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\CBAUATDeal_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{899B841B-C9B7-4EE3-857D-360D26F44E86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A8B2AC-DFCB-4090-94B5-1AD5F6160B6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2310" yWindow="3960" windowWidth="15705" windowHeight="8490" firstSheet="8" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SERV40_BreakFunding" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2506" uniqueCount="842">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2464" uniqueCount="842">
   <si>
     <t>rowid</t>
   </si>
@@ -2752,7 +2752,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2843,7 +2843,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3488,9 +3487,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AQ19"/>
+  <dimension ref="A1:AQ5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4181,167 +4182,6 @@
         <v>254</v>
       </c>
       <c r="AQ5" s="9" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
-      <c r="W6" t="s">
-        <v>506</v>
-      </c>
-      <c r="AQ6" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="D7" t="s">
-        <v>28</v>
-      </c>
-      <c r="W7" t="s">
-        <v>506</v>
-      </c>
-      <c r="AQ7" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="D8" t="s">
-        <v>28</v>
-      </c>
-      <c r="W8" t="s">
-        <v>506</v>
-      </c>
-      <c r="AQ8" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="D9" t="s">
-        <v>28</v>
-      </c>
-      <c r="W9" t="s">
-        <v>506</v>
-      </c>
-      <c r="AQ9" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="D10" t="s">
-        <v>28</v>
-      </c>
-      <c r="W10" t="s">
-        <v>506</v>
-      </c>
-      <c r="AQ10" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="D11" t="s">
-        <v>28</v>
-      </c>
-      <c r="W11" t="s">
-        <v>506</v>
-      </c>
-      <c r="AQ11" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="D12" t="s">
-        <v>28</v>
-      </c>
-      <c r="W12" t="s">
-        <v>506</v>
-      </c>
-      <c r="AQ12" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="D13" t="s">
-        <v>28</v>
-      </c>
-      <c r="W13" t="s">
-        <v>506</v>
-      </c>
-      <c r="AQ13" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="D14" t="s">
-        <v>28</v>
-      </c>
-      <c r="W14" t="s">
-        <v>506</v>
-      </c>
-      <c r="AQ14" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="D15" t="s">
-        <v>28</v>
-      </c>
-      <c r="W15" t="s">
-        <v>506</v>
-      </c>
-      <c r="AQ15" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="D16" t="s">
-        <v>28</v>
-      </c>
-      <c r="W16" t="s">
-        <v>506</v>
-      </c>
-      <c r="AQ16" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="17" spans="4:43" x14ac:dyDescent="0.2">
-      <c r="D17" t="s">
-        <v>28</v>
-      </c>
-      <c r="W17" t="s">
-        <v>506</v>
-      </c>
-      <c r="AQ17" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="18" spans="4:43" x14ac:dyDescent="0.2">
-      <c r="D18" t="s">
-        <v>28</v>
-      </c>
-      <c r="W18" t="s">
-        <v>506</v>
-      </c>
-      <c r="AB18" s="56"/>
-      <c r="AC18" s="56"/>
-      <c r="AD18" s="56"/>
-      <c r="AE18" s="56"/>
-      <c r="AF18" s="56"/>
-      <c r="AQ18" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="19" spans="4:43" x14ac:dyDescent="0.2">
-      <c r="D19" t="s">
-        <v>28</v>
-      </c>
-      <c r="W19" t="s">
-        <v>506</v>
-      </c>
-      <c r="AC19" s="9"/>
-      <c r="AF19" s="9"/>
-      <c r="AQ19" t="s">
         <v>357</v>
       </c>
     </row>
@@ -4659,80 +4499,80 @@
     <col min="25" max="25" width="19.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="57" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" s="56" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="56" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>624</v>
       </c>
-      <c r="D1" s="57" t="s">
+      <c r="D1" s="56" t="s">
         <v>537</v>
       </c>
-      <c r="E1" s="57" t="s">
+      <c r="E1" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="57" t="s">
+      <c r="F1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="57" t="s">
+      <c r="G1" s="56" t="s">
         <v>625</v>
       </c>
-      <c r="H1" s="57" t="s">
+      <c r="H1" s="56" t="s">
         <v>607</v>
       </c>
-      <c r="I1" s="57" t="s">
+      <c r="I1" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="57" t="s">
+      <c r="J1" s="56" t="s">
         <v>626</v>
       </c>
-      <c r="K1" s="57" t="s">
+      <c r="K1" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="57" t="s">
+      <c r="L1" s="56" t="s">
         <v>627</v>
       </c>
-      <c r="M1" s="57" t="s">
+      <c r="M1" s="56" t="s">
         <v>628</v>
       </c>
-      <c r="N1" s="57" t="s">
+      <c r="N1" s="56" t="s">
         <v>629</v>
       </c>
-      <c r="O1" s="57" t="s">
+      <c r="O1" s="56" t="s">
         <v>630</v>
       </c>
-      <c r="P1" s="57" t="s">
+      <c r="P1" s="56" t="s">
         <v>631</v>
       </c>
-      <c r="Q1" s="57" t="s">
+      <c r="Q1" s="56" t="s">
         <v>632</v>
       </c>
-      <c r="R1" s="57" t="s">
+      <c r="R1" s="56" t="s">
         <v>633</v>
       </c>
-      <c r="S1" s="57" t="s">
+      <c r="S1" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="57" t="s">
+      <c r="T1" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="U1" s="57" t="s">
+      <c r="U1" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="V1" s="57" t="s">
+      <c r="V1" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="W1" s="57" t="s">
+      <c r="W1" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="X1" s="57" t="s">
+      <c r="X1" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="Y1" s="57" t="s">
+      <c r="Y1" s="56" t="s">
         <v>634</v>
       </c>
     </row>
@@ -5208,7 +5048,7 @@
       </c>
     </row>
     <row r="8" spans="1:28" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="58" t="s">
+      <c r="A8" s="57" t="s">
         <v>393</v>
       </c>
       <c r="B8" s="9" t="s">
@@ -5229,7 +5069,7 @@
       <c r="G8" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="H8" s="59" t="s">
+      <c r="H8" s="58" t="s">
         <v>29</v>
       </c>
       <c r="I8" s="1" t="s">
@@ -5250,16 +5090,16 @@
       <c r="N8" s="10" t="s">
         <v>593</v>
       </c>
-      <c r="O8" s="59" t="s">
+      <c r="O8" s="58" t="s">
         <v>648</v>
       </c>
-      <c r="P8" s="59" t="s">
+      <c r="P8" s="58" t="s">
         <v>177</v>
       </c>
       <c r="Q8" s="10" t="s">
         <v>673</v>
       </c>
-      <c r="R8" s="59" t="s">
+      <c r="R8" s="58" t="s">
         <v>26</v>
       </c>
       <c r="S8" s="10" t="s">
@@ -5277,7 +5117,7 @@
       <c r="W8" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="X8" s="58" t="s">
+      <c r="X8" s="57" t="s">
         <v>36</v>
       </c>
       <c r="Y8" s="10" t="s">
@@ -5635,10 +5475,10 @@
       <c r="I1" s="21" t="s">
         <v>688</v>
       </c>
-      <c r="J1" s="60" t="s">
+      <c r="J1" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="60" t="s">
+      <c r="K1" s="59" t="s">
         <v>4</v>
       </c>
       <c r="L1" s="21" t="s">
@@ -6447,7 +6287,7 @@
       <c r="P3" s="9" t="s">
         <v>708</v>
       </c>
-      <c r="Q3" s="80" t="s">
+      <c r="Q3" s="79" t="s">
         <v>710</v>
       </c>
       <c r="R3" s="1" t="s">
@@ -6489,10 +6329,10 @@
       <c r="B1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="61" t="s">
+      <c r="C1" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="61" t="s">
+      <c r="D1" s="60" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="34" t="s">
@@ -6816,53 +6656,53 @@
     <col min="25" max="25" width="23.140625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="62" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+    <row r="1" spans="1:25" s="61" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="62" t="s">
+      <c r="D1" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="62" t="s">
+      <c r="E1" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="62" t="s">
+      <c r="F1" s="61" t="s">
         <v>699</v>
       </c>
-      <c r="G1" s="62" t="s">
+      <c r="G1" s="61" t="s">
         <v>720</v>
       </c>
-      <c r="H1" s="62" t="s">
+      <c r="H1" s="61" t="s">
         <v>721</v>
       </c>
-      <c r="I1" s="62" t="s">
+      <c r="I1" s="61" t="s">
         <v>722</v>
       </c>
-      <c r="J1" s="62" t="s">
+      <c r="J1" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="62" t="s">
+      <c r="K1" s="61" t="s">
         <v>723</v>
       </c>
-      <c r="L1" s="62" t="s">
+      <c r="L1" s="61" t="s">
         <v>724</v>
       </c>
-      <c r="M1" s="62" t="s">
+      <c r="M1" s="61" t="s">
         <v>725</v>
       </c>
-      <c r="N1" s="62" t="s">
+      <c r="N1" s="61" t="s">
         <v>726</v>
       </c>
-      <c r="O1" s="62" t="s">
+      <c r="O1" s="61" t="s">
         <v>727</v>
       </c>
-      <c r="P1" s="62" t="s">
+      <c r="P1" s="61" t="s">
         <v>16</v>
       </c>
       <c r="Q1" s="2" t="s">
@@ -6871,16 +6711,16 @@
       <c r="R1" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="S1" s="62" t="s">
+      <c r="S1" s="61" t="s">
         <v>728</v>
       </c>
-      <c r="T1" s="62" t="s">
+      <c r="T1" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="U1" s="62" t="s">
+      <c r="U1" s="61" t="s">
         <v>598</v>
       </c>
-      <c r="V1" s="62" t="s">
+      <c r="V1" s="61" t="s">
         <v>717</v>
       </c>
       <c r="W1" s="2" t="s">
@@ -6894,7 +6734,7 @@
       </c>
     </row>
     <row r="2" spans="1:25" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="62" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="9" t="s">
@@ -6971,7 +6811,7 @@
       </c>
     </row>
     <row r="3" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="62" t="s">
         <v>50</v>
       </c>
       <c r="B3" s="9" t="s">
@@ -6980,7 +6820,7 @@
       <c r="C3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="78" t="s">
+      <c r="D3" s="77" t="s">
         <v>736</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -7001,7 +6841,7 @@
       <c r="J3" s="15" t="s">
         <v>733</v>
       </c>
-      <c r="K3" s="78">
+      <c r="K3" s="77">
         <v>1</v>
       </c>
       <c r="L3" s="15" t="s">
@@ -7010,7 +6850,7 @@
       <c r="M3" s="9" t="s">
         <v>734</v>
       </c>
-      <c r="N3" s="78">
+      <c r="N3" s="77">
         <v>1</v>
       </c>
       <c r="O3" s="9" t="s">
@@ -7048,7 +6888,7 @@
       </c>
     </row>
     <row r="4" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="63" t="s">
+      <c r="A4" s="62" t="s">
         <v>194</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -7078,7 +6918,7 @@
       <c r="J4" s="15" t="s">
         <v>737</v>
       </c>
-      <c r="K4" s="78" t="s">
+      <c r="K4" s="77" t="s">
         <v>50</v>
       </c>
       <c r="L4" s="15" t="s">
@@ -7215,7 +7055,7 @@
       <c r="K17" s="40"/>
       <c r="L17" s="14"/>
       <c r="M17" s="40"/>
-      <c r="N17" s="79"/>
+      <c r="N17" s="78"/>
       <c r="O17" s="14"/>
     </row>
     <row r="18" spans="3:15" x14ac:dyDescent="0.25">
@@ -7383,7 +7223,7 @@
       <c r="G2" s="13" t="s">
         <v>747</v>
       </c>
-      <c r="H2" s="64" t="s">
+      <c r="H2" s="63" t="s">
         <v>187</v>
       </c>
       <c r="I2" s="1">
@@ -7404,7 +7244,7 @@
       <c r="N2" s="17" t="s">
         <v>527</v>
       </c>
-      <c r="O2" s="65">
+      <c r="O2" s="64">
         <v>7125114</v>
       </c>
       <c r="P2" s="18" t="s">
@@ -7475,7 +7315,7 @@
       <c r="G3" s="13" t="s">
         <v>747</v>
       </c>
-      <c r="H3" s="64" t="s">
+      <c r="H3" s="63" t="s">
         <v>187</v>
       </c>
       <c r="I3" s="1">
@@ -7496,7 +7336,7 @@
       <c r="N3" s="17" t="s">
         <v>649</v>
       </c>
-      <c r="O3" s="65">
+      <c r="O3" s="64">
         <v>7125114</v>
       </c>
       <c r="P3" s="18" t="s">
@@ -7567,7 +7407,7 @@
       <c r="G4" s="13" t="s">
         <v>747</v>
       </c>
-      <c r="H4" s="64" t="s">
+      <c r="H4" s="63" t="s">
         <v>187</v>
       </c>
       <c r="I4" s="1">
@@ -7588,7 +7428,7 @@
       <c r="N4" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="O4" s="65">
+      <c r="O4" s="64">
         <v>7125114</v>
       </c>
       <c r="P4" s="18" t="s">
@@ -7637,11 +7477,11 @@
       <c r="AU4" s="1"/>
       <c r="AV4" s="1"/>
     </row>
-    <row r="5" spans="1:48" s="66" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="67" t="s">
+    <row r="5" spans="1:48" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="66" t="s">
         <v>197</v>
       </c>
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="67" t="s">
         <v>746</v>
       </c>
       <c r="C5" s="10" t="s">
@@ -7650,49 +7490,49 @@
       <c r="D5" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="E5" s="67" t="s">
+      <c r="E5" s="66" t="s">
         <v>29</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>753</v>
       </c>
-      <c r="G5" s="67" t="s">
+      <c r="G5" s="66" t="s">
         <v>747</v>
       </c>
-      <c r="H5" s="69" t="s">
+      <c r="H5" s="68" t="s">
         <v>187</v>
       </c>
       <c r="I5" s="10">
         <v>7125114</v>
       </c>
-      <c r="J5" s="58" t="s">
+      <c r="J5" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="K5" s="67" t="s">
+      <c r="K5" s="66" t="s">
         <v>392</v>
       </c>
-      <c r="L5" s="66" t="s">
+      <c r="L5" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="M5" s="67" t="s">
+      <c r="M5" s="66" t="s">
         <v>754</v>
       </c>
-      <c r="N5" s="70" t="s">
+      <c r="N5" s="69" t="s">
         <v>527</v>
       </c>
-      <c r="O5" s="71">
+      <c r="O5" s="70">
         <v>7125114</v>
       </c>
-      <c r="P5" s="72" t="s">
+      <c r="P5" s="71" t="s">
         <v>42</v>
       </c>
       <c r="Q5" s="10" t="s">
         <v>648</v>
       </c>
-      <c r="R5" s="73" t="s">
+      <c r="R5" s="72" t="s">
         <v>749</v>
       </c>
-      <c r="S5" s="74" t="s">
+      <c r="S5" s="73" t="s">
         <v>755</v>
       </c>
       <c r="T5" s="10" t="s">
@@ -7751,7 +7591,7 @@
       <c r="G6" s="13" t="s">
         <v>747</v>
       </c>
-      <c r="H6" s="64" t="s">
+      <c r="H6" s="63" t="s">
         <v>187</v>
       </c>
       <c r="I6" s="1">
@@ -7772,7 +7612,7 @@
       <c r="N6" s="17" t="s">
         <v>649</v>
       </c>
-      <c r="O6" s="65">
+      <c r="O6" s="64">
         <v>7125114</v>
       </c>
       <c r="P6" s="18" t="s">
@@ -7843,7 +7683,7 @@
       <c r="G7" s="13" t="s">
         <v>747</v>
       </c>
-      <c r="H7" s="64" t="s">
+      <c r="H7" s="63" t="s">
         <v>187</v>
       </c>
       <c r="I7" s="1">
@@ -7864,7 +7704,7 @@
       <c r="N7" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="O7" s="65">
+      <c r="O7" s="64">
         <v>7125114</v>
       </c>
       <c r="P7" s="18" t="s">
@@ -7935,7 +7775,7 @@
       <c r="G8" s="13" t="s">
         <v>747</v>
       </c>
-      <c r="H8" s="64" t="s">
+      <c r="H8" s="63" t="s">
         <v>33</v>
       </c>
       <c r="I8" s="1">
@@ -7956,7 +7796,7 @@
       <c r="N8" s="17" t="s">
         <v>759</v>
       </c>
-      <c r="O8" s="65">
+      <c r="O8" s="64">
         <v>7125114</v>
       </c>
       <c r="P8" s="18" t="s">
@@ -8038,7 +7878,7 @@
       <c r="N9" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="O9" s="65">
+      <c r="O9" s="64">
         <v>7125114</v>
       </c>
       <c r="P9" s="18" t="s">
@@ -8097,7 +7937,7 @@
       <c r="N10" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="O10" s="65">
+      <c r="O10" s="64">
         <v>7125114</v>
       </c>
       <c r="P10" s="18" t="s">
@@ -8152,13 +7992,13 @@
       <c r="C18" t="s">
         <v>28</v>
       </c>
-      <c r="I18" s="75"/>
+      <c r="I18" s="74"/>
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>28</v>
       </c>
-      <c r="I19" s="75"/>
+      <c r="I19" s="74"/>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
@@ -8170,28 +8010,28 @@
         <v>28</v>
       </c>
       <c r="D21" s="1"/>
-      <c r="I21" s="75"/>
+      <c r="I21" s="74"/>
     </row>
     <row r="22" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>28</v>
       </c>
       <c r="D22" s="1"/>
-      <c r="I22" s="75"/>
+      <c r="I22" s="74"/>
     </row>
     <row r="23" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>28</v>
       </c>
       <c r="D23" s="1"/>
-      <c r="I23" s="75"/>
+      <c r="I23" s="74"/>
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>28</v>
       </c>
       <c r="D24" s="1"/>
-      <c r="I24" s="75"/>
+      <c r="I24" s="74"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
@@ -8393,10 +8233,10 @@
       <c r="E2" t="s">
         <v>769</v>
       </c>
-      <c r="F2" s="76" t="s">
+      <c r="F2" s="75" t="s">
         <v>575</v>
       </c>
-      <c r="G2" s="76" t="s">
+      <c r="G2" s="75" t="s">
         <v>575</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -8449,10 +8289,10 @@
       <c r="E3" s="1" t="s">
         <v>769</v>
       </c>
-      <c r="F3" s="76" t="s">
+      <c r="F3" s="75" t="s">
         <v>575</v>
       </c>
-      <c r="G3" s="76" t="s">
+      <c r="G3" s="75" t="s">
         <v>575</v>
       </c>
       <c r="H3" s="1" t="s">
@@ -8484,10 +8324,10 @@
       <c r="E4" s="1" t="s">
         <v>769</v>
       </c>
-      <c r="F4" s="76" t="s">
+      <c r="F4" s="75" t="s">
         <v>575</v>
       </c>
-      <c r="G4" s="76" t="s">
+      <c r="G4" s="75" t="s">
         <v>575</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -8519,10 +8359,10 @@
       <c r="E5" s="1" t="s">
         <v>769</v>
       </c>
-      <c r="F5" s="76" t="s">
+      <c r="F5" s="75" t="s">
         <v>575</v>
       </c>
-      <c r="G5" s="76" t="s">
+      <c r="G5" s="75" t="s">
         <v>575</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -8662,7 +8502,7 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="77" t="s">
+      <c r="A3" s="76" t="s">
         <v>50</v>
       </c>
       <c r="B3" s="9" t="s">
@@ -8695,7 +8535,7 @@
       <c r="K3" s="9" t="s">
         <v>772</v>
       </c>
-      <c r="L3" s="65">
+      <c r="L3" s="64">
         <v>7125114</v>
       </c>
       <c r="M3" s="9" t="s">
@@ -8706,7 +8546,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="76" t="s">
         <v>194</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -8739,7 +8579,7 @@
       <c r="K4" s="9" t="s">
         <v>772</v>
       </c>
-      <c r="L4" s="65">
+      <c r="L4" s="64">
         <v>7125114</v>
       </c>
       <c r="M4" s="9" t="s">
@@ -8750,7 +8590,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="77" t="s">
+      <c r="A5" s="76" t="s">
         <v>197</v>
       </c>
       <c r="B5" s="9" t="s">
@@ -8783,7 +8623,7 @@
       <c r="K5" s="9" t="s">
         <v>772</v>
       </c>
-      <c r="L5" s="65">
+      <c r="L5" s="64">
         <v>7125114</v>
       </c>
       <c r="M5" s="9" t="s">
@@ -9153,7 +8993,7 @@
       <c r="E2" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F2" s="81" t="s">
+      <c r="F2" s="80" t="s">
         <v>839</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -11522,8 +11362,8 @@
   </sheetPr>
   <dimension ref="A1:BS28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11826,7 +11666,7 @@
       <c r="D2" s="50" t="s">
         <v>348</v>
       </c>
-      <c r="E2" s="81" t="s">
+      <c r="E2" s="80" t="s">
         <v>841</v>
       </c>
       <c r="F2" s="51" t="s">
@@ -12677,7 +12517,9 @@
   </sheetPr>
   <dimension ref="A1:BP6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
GDE-6716 - Updates after final run
</commit_message>
<xml_diff>
--- a/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT03.xlsx
+++ b/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT03.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\CBAUATDeal_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A8B2AC-DFCB-4090-94B5-1AD5F6160B6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87CEBAB7-E808-4DCD-9226-74699F11E1B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2310" yWindow="3960" windowWidth="15705" windowHeight="8490" firstSheet="8" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SERV40_BreakFunding" sheetId="1" r:id="rId1"/>
@@ -2562,13 +2562,13 @@
     <t>CUSTSHORT11112</t>
   </si>
   <si>
-    <t>1813410</t>
-  </si>
-  <si>
     <t>CTBAAU2SXXX</t>
   </si>
   <si>
-    <t>0813410</t>
+    <t>1413932</t>
+  </si>
+  <si>
+    <t>1414010</t>
   </si>
 </sst>
 </file>
@@ -3203,7 +3203,9 @@
   </sheetPr>
   <dimension ref="A1:Z3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3489,7 +3491,7 @@
   </sheetPr>
   <dimension ref="A1:AQ5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -8713,8 +8715,8 @@
   <dimension ref="A1:CP2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C19" sqref="C19"/>
+      <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8994,7 +8996,7 @@
         <v>96</v>
       </c>
       <c r="F2" s="80" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>96</v>
@@ -11362,8 +11364,8 @@
   </sheetPr>
   <dimension ref="A1:BS28"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11838,7 +11840,7 @@
         <v>387</v>
       </c>
       <c r="BJ2" s="1" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="BK2" s="1" t="s">
         <v>96</v>
@@ -11932,7 +11934,7 @@
         <v>387</v>
       </c>
       <c r="BJ5" s="1" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="BK5" s="1" t="s">
         <v>96</v>
@@ -12518,7 +12520,7 @@
   <dimension ref="A1:BP6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Last commmit before transferring to new branch
</commit_message>
<xml_diff>
--- a/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT03.xlsx
+++ b/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT03.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\CBAUATDeal_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECBEA3F4-89DA-40AF-BEB6-C1B587F8569C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9EF9791-2049-4382-902C-77E55B4E20C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PTY001_QuickPartyOnboarding (2)" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2573" uniqueCount="855">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2573" uniqueCount="854">
   <si>
     <t>rowid</t>
   </si>
@@ -2610,9 +2610,6 @@
   </si>
   <si>
     <t>to the actual due date</t>
-  </si>
-  <si>
-    <t>28-Nov-2019</t>
   </si>
   <si>
     <t>Fee_Type</t>
@@ -12411,7 +12408,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12442,7 +12439,7 @@
         <v>76</v>
       </c>
       <c r="E1" s="88" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="F1" s="87" t="s">
         <v>281</v>
@@ -12473,7 +12470,7 @@
       <c r="D2" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="9" t="s">
         <v>179</v>
       </c>
       <c r="F2" s="85" t="s">
@@ -12505,11 +12502,11 @@
       <c r="D3" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="9" t="s">
         <v>179</v>
       </c>
       <c r="F3" s="85" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="G3" s="77" t="s">
         <v>850</v>
@@ -12537,11 +12534,11 @@
       <c r="D4" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="9" t="s">
         <v>179</v>
       </c>
       <c r="F4" s="85" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="G4" s="77" t="s">
         <v>850</v>
@@ -12569,7 +12566,7 @@
       <c r="D5" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="9" t="s">
         <v>200</v>
       </c>
       <c r="F5" s="85" t="s">
@@ -12579,7 +12576,7 @@
         <v>662</v>
       </c>
       <c r="H5" s="85" t="s">
-        <v>852</v>
+        <v>282</v>
       </c>
       <c r="I5" t="s">
         <v>712</v>

</xml_diff>

<commit_message>
GDE-6891 Update Generic Keywords and EVG_CBAUAT03.xlsx and IEE.py
</commit_message>
<xml_diff>
--- a/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT03.xlsx
+++ b/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT03.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\CBAUATDeal_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3239A4CD-F3C1-4215-80A6-7330BDF6617F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F4B4891-C65C-4B62-A4C5-3464FA7724D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="15" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6996,14 +6996,14 @@
   <dimension ref="A1:Y20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="26.5703125" style="1" customWidth="1"/>
     <col min="6" max="10" width="23.28515625" style="1" customWidth="1"/>

</xml_diff>

<commit_message>
GDE-6998 Update Extend Maturity and Limit for FCAF
</commit_message>
<xml_diff>
--- a/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT03.xlsx
+++ b/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT03.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\CBAUATDeal_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5B938A-0F62-402B-8BDD-0475C3A013AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A0F0CE-EAD2-4667-8823-65E35FC64F5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5355" yWindow="1575" windowWidth="21600" windowHeight="11385" firstSheet="17" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="17" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SERV40_BreakFunding" sheetId="1" r:id="rId1"/>
@@ -8577,7 +8577,7 @@
   <dimension ref="A1:CJ5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8810,19 +8810,19 @@
         <v>364</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>195</v>
+        <v>778</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>804</v>
       </c>
       <c r="F3" s="70" t="s">
-        <v>591</v>
+        <v>600</v>
       </c>
       <c r="G3" s="70" t="s">
-        <v>591</v>
+        <v>600</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>805</v>
@@ -8845,19 +8845,19 @@
         <v>364</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>52</v>
+        <v>780</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>804</v>
       </c>
       <c r="F4" s="70" t="s">
-        <v>591</v>
+        <v>600</v>
       </c>
       <c r="G4" s="70" t="s">
-        <v>591</v>
+        <v>600</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>805</v>
@@ -8880,19 +8880,19 @@
         <v>364</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>202</v>
+        <v>31</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>804</v>
       </c>
       <c r="F5" s="70" t="s">
-        <v>591</v>
+        <v>608</v>
       </c>
       <c r="G5" s="70" t="s">
-        <v>591</v>
+        <v>608</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>805</v>
@@ -9324,7 +9324,7 @@
   <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9440,13 +9440,13 @@
         <v>364</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>203</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>195</v>
+        <v>778</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>813</v>
@@ -9484,13 +9484,13 @@
         <v>364</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>203</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>52</v>
+        <v>780</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>813</v>
@@ -9528,13 +9528,13 @@
         <v>364</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>203</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>202</v>
+        <v>31</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>813</v>

</xml_diff>

<commit_message>
GDE-6998 - February 01, 2019 - AMCH05 - FCAF - Facility Extension and Limit Increase | AU | 1.00 GDE-6999 - February 01, 2019 - AMCH05 - FCAF - Extension Fee Setup and Collection | AU | 1.0 GDE-7000 - February 01, 2019 - AMCH05 - SCAF - Facility Extension and Limit Increase | AU | 3.75 GDE-7001 - February 01, 2019 - AMCH05 - SCAF - Extension Fee Setup and Collection | AU | 1.00 GDE-7003 - February 01, 2019 - AMCH05 - TCAF - Extension Fee Setup and Collection | AU | 1.00
</commit_message>
<xml_diff>
--- a/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT03.xlsx
+++ b/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT03.xlsx
@@ -8,39 +8,40 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\CBAUATDeal_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A0F0CE-EAD2-4667-8823-65E35FC64F5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA31923-8AD2-4B23-9FF5-0C806AB30038}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="17" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="16" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SERV40_BreakFunding" sheetId="1" r:id="rId1"/>
     <sheet name="PTY001_QuickPartyOnboarding" sheetId="2" state="hidden" r:id="rId2"/>
     <sheet name="FXRates_Fields" sheetId="4" r:id="rId3"/>
-    <sheet name="CRED01_Primaries" sheetId="5" r:id="rId4"/>
-    <sheet name="BaseRate_Fields" sheetId="6" r:id="rId5"/>
-    <sheet name="CRED08_OngoingFeeSetup" sheetId="7" r:id="rId6"/>
-    <sheet name="ORIG03_Customer" sheetId="8" r:id="rId7"/>
-    <sheet name="CRED01_DealSetup" sheetId="9" r:id="rId8"/>
-    <sheet name="CRED02_FacilitySetup" sheetId="10" r:id="rId9"/>
-    <sheet name="SERV05_SBLCIssuance" sheetId="11" r:id="rId10"/>
-    <sheet name="SERV01_LoanDrawdown" sheetId="12" r:id="rId11"/>
-    <sheet name="SERV18_FeeOnLenderSharesPayment" sheetId="13" r:id="rId12"/>
-    <sheet name="SERV29_LineFeePayment" sheetId="14" r:id="rId13"/>
-    <sheet name="SERV29_CommitmentFeePayment" sheetId="15" r:id="rId14"/>
-    <sheet name="PTY001_QuickPartyOnboarding (2)" sheetId="16" r:id="rId15"/>
-    <sheet name="SERV23_Paperclip" sheetId="17" r:id="rId16"/>
-    <sheet name="SERV08C_ComprehensiveRepricing" sheetId="18" r:id="rId17"/>
-    <sheet name="CRED08_FacilityFeeSetup" sheetId="3" r:id="rId18"/>
-    <sheet name="AMCH05_ExtendFacility" sheetId="19" r:id="rId19"/>
-    <sheet name="CRED01_UpfrontFee" sheetId="20" r:id="rId20"/>
-    <sheet name="COM06_LoanMerge" sheetId="21" r:id="rId21"/>
+    <sheet name="AMCH06_PricingChangeTransaction" sheetId="22" r:id="rId4"/>
+    <sheet name="CRED01_Primaries" sheetId="5" r:id="rId5"/>
+    <sheet name="BaseRate_Fields" sheetId="6" r:id="rId6"/>
+    <sheet name="CRED08_OngoingFeeSetup" sheetId="7" r:id="rId7"/>
+    <sheet name="ORIG03_Customer" sheetId="8" r:id="rId8"/>
+    <sheet name="CRED01_DealSetup" sheetId="9" r:id="rId9"/>
+    <sheet name="CRED02_FacilitySetup" sheetId="10" r:id="rId10"/>
+    <sheet name="SERV05_SBLCIssuance" sheetId="11" r:id="rId11"/>
+    <sheet name="SERV01_LoanDrawdown" sheetId="12" r:id="rId12"/>
+    <sheet name="SERV18_FeeOnLenderSharesPayment" sheetId="13" r:id="rId13"/>
+    <sheet name="SERV29_LineFeePayment" sheetId="14" r:id="rId14"/>
+    <sheet name="SERV29_CommitmentFeePayment" sheetId="15" r:id="rId15"/>
+    <sheet name="PTY001_QuickPartyOnboarding (2)" sheetId="16" r:id="rId16"/>
+    <sheet name="SERV23_Paperclip" sheetId="17" r:id="rId17"/>
+    <sheet name="SERV08C_ComprehensiveRepricing" sheetId="18" r:id="rId18"/>
+    <sheet name="CRED08_FacilityFeeSetup" sheetId="3" r:id="rId19"/>
+    <sheet name="AMCH05_ExtendFacility" sheetId="19" r:id="rId20"/>
+    <sheet name="CRED01_UpfrontFee" sheetId="20" r:id="rId21"/>
+    <sheet name="COM06_LoanMerge" sheetId="21" r:id="rId22"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2580" uniqueCount="874">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2662" uniqueCount="930">
   <si>
     <t>rowid</t>
   </si>
@@ -2666,16 +2667,185 @@
   </si>
   <si>
     <t>CUSTSHORT11112</t>
+  </si>
+  <si>
+    <t>Pricing_Status</t>
+  </si>
+  <si>
+    <t>TransactionNo_Prefix</t>
+  </si>
+  <si>
+    <t>PricingChange_TransactionNo</t>
+  </si>
+  <si>
+    <t>PricingChange_EffectiveDate</t>
+  </si>
+  <si>
+    <t>PricingChange_Desc</t>
+  </si>
+  <si>
+    <t>OngoingFeeItem</t>
+  </si>
+  <si>
+    <t>OngoingFeeType</t>
+  </si>
+  <si>
+    <t>OngoingFeeItemAfter</t>
+  </si>
+  <si>
+    <t>FormulaCategoryType</t>
+  </si>
+  <si>
+    <t>OngoingFeePercent</t>
+  </si>
+  <si>
+    <t>RateBasis</t>
+  </si>
+  <si>
+    <t>UnutilizedRate</t>
+  </si>
+  <si>
+    <t>FeeString</t>
+  </si>
+  <si>
+    <t>Facility_OngoingFeeRateStr</t>
+  </si>
+  <si>
+    <t>Facility_OngoingFeeRate_SavedStr</t>
+  </si>
+  <si>
+    <t>PricingChange_OngoingFeeRate</t>
+  </si>
+  <si>
+    <t>PricingChange_OngoingFeeRate_SavedStr</t>
+  </si>
+  <si>
+    <t>AvailablePricing_Window</t>
+  </si>
+  <si>
+    <t>FeeSelection_Window</t>
+  </si>
+  <si>
+    <t>Approval_Question</t>
+  </si>
+  <si>
+    <t>Release_Status</t>
+  </si>
+  <si>
+    <t>Created_Event</t>
+  </si>
+  <si>
+    <t>OngoingFeePricingChanged_Event</t>
+  </si>
+  <si>
+    <t>SentToApproval_Event</t>
+  </si>
+  <si>
+    <t>Approved_Event</t>
+  </si>
+  <si>
+    <t>Released_Event</t>
+  </si>
+  <si>
+    <t>OngoingFeeRate_Original</t>
+  </si>
+  <si>
+    <t>OngoingFeeRate_SaveOriginal</t>
+  </si>
+  <si>
+    <t>PricingChangeSheet</t>
+  </si>
+  <si>
+    <t>PricingChange_OngoingFeeStr</t>
+  </si>
+  <si>
+    <t>Interest_AddItem</t>
+  </si>
+  <si>
+    <t>Interest_RateBasis</t>
+  </si>
+  <si>
+    <t>Interest_SpreadAmt1</t>
+  </si>
+  <si>
+    <t>EVG_PTYLIQ01 Scenario1 Baseline Bilateral</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>TRN02</t>
+  </si>
+  <si>
+    <t>5%</t>
+  </si>
+  <si>
+    <t>Ongoing Fee String</t>
+  </si>
+  <si>
+    <t>${SPACE}${SPACE}${SPACE}${SPACE}Unutilized X Rate (5%)</t>
+  </si>
+  <si>
+    <t>Available Pricing</t>
+  </si>
+  <si>
+    <t>Fee Selection</t>
+  </si>
+  <si>
+    <t>Are you sure you want to approve this transaction?</t>
+  </si>
+  <si>
+    <t>Release</t>
+  </si>
+  <si>
+    <t>Created</t>
+  </si>
+  <si>
+    <t>Ongoing Fee Pricing Changed</t>
+  </si>
+  <si>
+    <t>Sent to Approval</t>
+  </si>
+  <si>
+    <t>Released</t>
+  </si>
+  <si>
+    <t>${SPACE}${SPACE}${SPACE}${SPACE}Unutilized X Rate (4%)</t>
+  </si>
+  <si>
+    <t>4%</t>
+  </si>
+  <si>
+    <t>Pricing_Change_Transaction</t>
+  </si>
+  <si>
+    <t>Basis Points</t>
+  </si>
+  <si>
+    <t>Commitment Fee Change</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>0.55</t>
+  </si>
+  <si>
+    <t>0.55%</t>
+  </si>
+  <si>
+    <t>${SPACE}${SPACE}${SPACE}${SPACE}Unutilized X Rate (0.525%)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d/yy"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2739,6 +2909,13 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -2877,7 +3054,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -3020,6 +3197,25 @@
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3629,6 +3825,716 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:AQ5"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17" style="1" customWidth="1"/>
+    <col min="8" max="8" width="24.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="23.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="20.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="23.140625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="31.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="18" style="1" customWidth="1"/>
+    <col min="17" max="17" width="21.5703125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="21.7109375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="26.5703125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="19.42578125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="32.7109375" style="1" customWidth="1"/>
+    <col min="22" max="22" width="21" style="1" customWidth="1"/>
+    <col min="23" max="23" width="18.28515625" style="1" customWidth="1"/>
+    <col min="24" max="24" width="20" style="1" customWidth="1"/>
+    <col min="25" max="26" width="19.85546875" style="1" customWidth="1"/>
+    <col min="27" max="28" width="25.85546875" style="1" customWidth="1"/>
+    <col min="29" max="30" width="26.5703125" style="1" customWidth="1"/>
+    <col min="31" max="32" width="25.5703125" style="1" customWidth="1"/>
+    <col min="33" max="34" width="26.85546875" style="1" customWidth="1"/>
+    <col min="35" max="37" width="14.85546875" style="1" customWidth="1"/>
+    <col min="38" max="39" width="20.42578125" style="1" customWidth="1"/>
+    <col min="40" max="41" width="33" style="1" customWidth="1"/>
+    <col min="42" max="43" width="16.85546875" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:43" s="28" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>550</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>460</v>
+      </c>
+      <c r="G1" s="28" t="s">
+        <v>551</v>
+      </c>
+      <c r="H1" s="28" t="s">
+        <v>552</v>
+      </c>
+      <c r="I1" s="28" t="s">
+        <v>553</v>
+      </c>
+      <c r="J1" s="28" t="s">
+        <v>554</v>
+      </c>
+      <c r="K1" s="28" t="s">
+        <v>555</v>
+      </c>
+      <c r="L1" s="28" t="s">
+        <v>556</v>
+      </c>
+      <c r="M1" s="28" t="s">
+        <v>557</v>
+      </c>
+      <c r="N1" s="28" t="s">
+        <v>558</v>
+      </c>
+      <c r="O1" s="28" t="s">
+        <v>559</v>
+      </c>
+      <c r="P1" s="28" t="s">
+        <v>560</v>
+      </c>
+      <c r="Q1" s="28" t="s">
+        <v>561</v>
+      </c>
+      <c r="R1" s="28" t="s">
+        <v>562</v>
+      </c>
+      <c r="S1" s="28" t="s">
+        <v>563</v>
+      </c>
+      <c r="T1" s="28" t="s">
+        <v>564</v>
+      </c>
+      <c r="U1" s="28" t="s">
+        <v>565</v>
+      </c>
+      <c r="V1" s="28" t="s">
+        <v>566</v>
+      </c>
+      <c r="W1" s="28" t="s">
+        <v>567</v>
+      </c>
+      <c r="X1" s="28" t="s">
+        <v>568</v>
+      </c>
+      <c r="Y1" s="28" t="s">
+        <v>569</v>
+      </c>
+      <c r="Z1" s="28" t="s">
+        <v>570</v>
+      </c>
+      <c r="AA1" s="28" t="s">
+        <v>571</v>
+      </c>
+      <c r="AB1" s="28" t="s">
+        <v>572</v>
+      </c>
+      <c r="AC1" s="28" t="s">
+        <v>573</v>
+      </c>
+      <c r="AD1" s="28" t="s">
+        <v>574</v>
+      </c>
+      <c r="AE1" s="28" t="s">
+        <v>575</v>
+      </c>
+      <c r="AF1" s="28" t="s">
+        <v>576</v>
+      </c>
+      <c r="AG1" s="28" t="s">
+        <v>577</v>
+      </c>
+      <c r="AH1" s="28" t="s">
+        <v>578</v>
+      </c>
+      <c r="AI1" s="28" t="s">
+        <v>579</v>
+      </c>
+      <c r="AJ1" s="28" t="s">
+        <v>580</v>
+      </c>
+      <c r="AK1" s="28" t="s">
+        <v>581</v>
+      </c>
+      <c r="AL1" s="28" t="s">
+        <v>582</v>
+      </c>
+      <c r="AM1" s="28" t="s">
+        <v>583</v>
+      </c>
+      <c r="AN1" s="28" t="s">
+        <v>584</v>
+      </c>
+      <c r="AO1" s="28" t="s">
+        <v>585</v>
+      </c>
+      <c r="AP1" s="28" t="s">
+        <v>586</v>
+      </c>
+      <c r="AQ1" s="28" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="2" spans="1:43" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>588</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>589</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>590</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>591</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="P2" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="R2" s="12" t="s">
+        <v>593</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>594</v>
+      </c>
+      <c r="T2" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="U2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="V2" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="X2" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y2" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z2" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="AA2" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="AB2" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="AE2" s="9" t="s">
+        <v>596</v>
+      </c>
+      <c r="AF2" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="AG2" s="9" t="s">
+        <v>597</v>
+      </c>
+      <c r="AH2" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="AI2" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ2" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="AK2" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="AL2" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="AM2" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="AN2" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="AO2" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="AP2" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="AQ2" s="9" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="3" spans="1:43" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>598</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>599</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>591</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>600</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="O3" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q3" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="R3" s="12" t="s">
+        <v>593</v>
+      </c>
+      <c r="S3" s="9" t="s">
+        <v>594</v>
+      </c>
+      <c r="T3" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="U3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="V3" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="X3" s="9" t="s">
+        <v>601</v>
+      </c>
+      <c r="Y3" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z3" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="AA3" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="AB3" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="AE3" s="9" t="s">
+        <v>596</v>
+      </c>
+      <c r="AF3" s="9" t="s">
+        <v>596</v>
+      </c>
+      <c r="AG3" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="AH3" s="9" t="s">
+        <v>597</v>
+      </c>
+      <c r="AI3" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ3" s="9" t="s">
+        <v>414</v>
+      </c>
+      <c r="AK3" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="AL3" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="AM3" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="AN3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AO3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AP3" s="9" t="s">
+        <v>526</v>
+      </c>
+      <c r="AQ3" s="9" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:43" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>603</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>599</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>604</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>605</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>606</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q4" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="R4" s="12" t="s">
+        <v>593</v>
+      </c>
+      <c r="S4" s="9" t="s">
+        <v>594</v>
+      </c>
+      <c r="T4" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="U4" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="V4" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="X4" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y4" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z4" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="AA4" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="AB4" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="AE4" s="9" t="s">
+        <v>596</v>
+      </c>
+      <c r="AF4" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="AG4" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="AH4" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="AI4" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ4" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="AK4" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="AL4" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="AM4" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="AN4" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AO4" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="AP4" s="9" t="s">
+        <v>526</v>
+      </c>
+      <c r="AQ4" s="9" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>607</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>599</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>604</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>600</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>608</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="O5" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="P5" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q5" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="R5" s="12" t="s">
+        <v>593</v>
+      </c>
+      <c r="S5" s="9" t="s">
+        <v>594</v>
+      </c>
+      <c r="T5" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="U5" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="V5" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="X5" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y5" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z5" s="9" t="s">
+        <v>414</v>
+      </c>
+      <c r="AA5" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="AB5" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="AE5" s="9" t="s">
+        <v>596</v>
+      </c>
+      <c r="AF5" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="AG5" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="AH5" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="AI5" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ5" s="9" t="s">
+        <v>414</v>
+      </c>
+      <c r="AK5" s="9" t="s">
+        <v>426</v>
+      </c>
+      <c r="AL5" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="AM5" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="AN5" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AO5" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="AP5" s="9" t="s">
+        <v>526</v>
+      </c>
+      <c r="AQ5" s="9" t="s">
+        <v>375</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
+  <pageSetup paperSize="9" pageOrder="overThenDown" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -3897,7 +4803,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -4765,7 +5671,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -5446,7 +6352,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -5663,7 +6569,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -5921,7 +6827,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -6323,7 +7229,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -6804,7 +7710,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -7729,7 +8635,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -8560,351 +9466,6 @@
       </c>
       <c r="AZ5" s="1" t="s">
         <v>194</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
-  <pageSetup paperSize="9" pageOrder="overThenDown" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:CJ5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="6.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="60.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="32.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.5703125" style="1" customWidth="1"/>
-    <col min="6" max="7" width="22.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="22.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="26.140625" style="1" customWidth="1"/>
-    <col min="11" max="35" width="22.28515625" style="1" customWidth="1"/>
-    <col min="36" max="36" width="28.85546875" style="1" customWidth="1"/>
-    <col min="37" max="37" width="14.28515625" style="1" customWidth="1"/>
-    <col min="38" max="38" width="23" style="1" customWidth="1"/>
-    <col min="39" max="42" width="19.85546875" style="1" customWidth="1"/>
-    <col min="43" max="44" width="24.7109375" style="1" customWidth="1"/>
-    <col min="45" max="45" width="25" style="1" customWidth="1"/>
-    <col min="46" max="46" width="24.42578125" style="1" customWidth="1"/>
-    <col min="47" max="47" width="30.42578125" style="1" customWidth="1"/>
-    <col min="48" max="48" width="36" style="1" customWidth="1"/>
-    <col min="49" max="49" width="34.42578125" style="1" customWidth="1"/>
-    <col min="50" max="50" width="26.7109375" style="1" customWidth="1"/>
-    <col min="51" max="52" width="17.28515625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="34.140625" style="1" customWidth="1"/>
-    <col min="54" max="54" width="28.42578125" style="1" customWidth="1"/>
-    <col min="55" max="55" width="24.7109375" style="1" customWidth="1"/>
-    <col min="56" max="56" width="30.28515625" style="1" customWidth="1"/>
-    <col min="57" max="57" width="17.5703125" style="1" customWidth="1"/>
-    <col min="58" max="58" width="20.28515625" style="1" customWidth="1"/>
-    <col min="59" max="59" width="12.140625" style="1" customWidth="1"/>
-    <col min="60" max="60" width="21.42578125" style="1" customWidth="1"/>
-    <col min="61" max="61" width="24.140625" style="1" customWidth="1"/>
-    <col min="62" max="62" width="16" style="1" customWidth="1"/>
-    <col min="63" max="63" width="14" style="1" customWidth="1"/>
-    <col min="64" max="64" width="16.7109375" style="1" customWidth="1"/>
-    <col min="65" max="65" width="10.42578125" style="1" customWidth="1"/>
-    <col min="66" max="66" width="37.7109375" style="1" customWidth="1"/>
-    <col min="67" max="68" width="16.7109375" style="1" customWidth="1"/>
-    <col min="69" max="71" width="20.140625" style="1" customWidth="1"/>
-    <col min="72" max="72" width="17.7109375" style="1" customWidth="1"/>
-    <col min="73" max="73" width="24.5703125" style="1" customWidth="1"/>
-    <col min="74" max="76" width="19.42578125" style="1" customWidth="1"/>
-    <col min="77" max="77" width="21.140625" style="1" customWidth="1"/>
-    <col min="78" max="78" width="32.42578125" style="1" customWidth="1"/>
-    <col min="79" max="80" width="17.28515625" style="1" customWidth="1"/>
-    <col min="81" max="83" width="17.5703125" style="1" customWidth="1"/>
-    <col min="84" max="84" width="26.28515625" style="1" customWidth="1"/>
-    <col min="85" max="85" width="35" style="1" customWidth="1"/>
-    <col min="86" max="86" width="26.5703125" style="1" customWidth="1"/>
-    <col min="87" max="87" width="24.85546875" style="1" customWidth="1"/>
-    <col min="88" max="88" width="20" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:88" s="19" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>799</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>616</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>800</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>801</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>802</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>803</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>619</v>
-      </c>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
-      <c r="AB1" s="3"/>
-      <c r="AC1" s="3"/>
-      <c r="AD1" s="3"/>
-      <c r="AE1" s="3"/>
-      <c r="AF1" s="3"/>
-      <c r="AG1" s="3"/>
-      <c r="AH1" s="3"/>
-      <c r="AI1" s="3"/>
-      <c r="AJ1" s="3"/>
-      <c r="AK1" s="3"/>
-      <c r="AL1" s="3"/>
-      <c r="AM1" s="3"/>
-      <c r="AN1" s="3"/>
-      <c r="AO1" s="3"/>
-      <c r="AP1" s="3"/>
-      <c r="AQ1" s="3"/>
-      <c r="AR1" s="3"/>
-      <c r="AS1" s="3"/>
-      <c r="AT1" s="3"/>
-      <c r="AU1" s="3"/>
-      <c r="AV1" s="3"/>
-      <c r="AW1" s="3"/>
-      <c r="AX1" s="3"/>
-      <c r="AY1" s="3"/>
-      <c r="AZ1" s="3"/>
-      <c r="BA1" s="3"/>
-      <c r="BB1" s="3"/>
-      <c r="BC1" s="3"/>
-      <c r="BD1" s="3"/>
-      <c r="BE1" s="3"/>
-      <c r="BF1" s="3"/>
-      <c r="BG1" s="3"/>
-      <c r="BH1" s="3"/>
-      <c r="BI1" s="3"/>
-      <c r="BJ1" s="3"/>
-      <c r="BK1" s="3"/>
-      <c r="BL1" s="3"/>
-      <c r="BM1" s="3"/>
-      <c r="BN1" s="3"/>
-      <c r="BO1" s="3"/>
-      <c r="BP1" s="3"/>
-      <c r="BQ1" s="3"/>
-      <c r="BR1" s="3"/>
-      <c r="BS1" s="3"/>
-      <c r="BT1" s="3"/>
-      <c r="BU1" s="3"/>
-      <c r="BV1" s="3"/>
-      <c r="BW1" s="3"/>
-      <c r="BX1" s="3"/>
-      <c r="BY1" s="3"/>
-      <c r="BZ1" s="3"/>
-      <c r="CA1" s="3"/>
-      <c r="CB1" s="3"/>
-      <c r="CC1" s="3"/>
-      <c r="CD1" s="3"/>
-      <c r="CE1" s="3"/>
-      <c r="CF1" s="3"/>
-      <c r="CG1" s="3"/>
-      <c r="CH1" s="3"/>
-      <c r="CI1" s="3"/>
-      <c r="CJ1" s="3"/>
-    </row>
-    <row r="2" spans="1:88" x14ac:dyDescent="0.2">
-      <c r="A2" s="82" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>773</v>
-      </c>
-      <c r="E2" t="s">
-        <v>804</v>
-      </c>
-      <c r="F2" s="70" t="s">
-        <v>591</v>
-      </c>
-      <c r="G2" s="70" t="s">
-        <v>591</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>805</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>782</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>806</v>
-      </c>
-      <c r="K2" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="22"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="23"/>
-      <c r="U2" s="11"/>
-      <c r="V2" s="11"/>
-      <c r="W2" s="24"/>
-      <c r="X2" s="24"/>
-      <c r="Y2" s="24"/>
-      <c r="Z2" s="25"/>
-      <c r="AA2" s="25"/>
-      <c r="AB2" s="24"/>
-      <c r="AC2" s="24"/>
-      <c r="AD2" s="24"/>
-      <c r="AE2" s="11"/>
-      <c r="AF2" s="11"/>
-    </row>
-    <row r="3" spans="1:88" x14ac:dyDescent="0.2">
-      <c r="A3" s="82" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>778</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>804</v>
-      </c>
-      <c r="F3" s="70" t="s">
-        <v>600</v>
-      </c>
-      <c r="G3" s="70" t="s">
-        <v>600</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>805</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>806</v>
-      </c>
-      <c r="K3" s="22" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:88" x14ac:dyDescent="0.2">
-      <c r="A4" s="82" t="s">
-        <v>198</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>780</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>804</v>
-      </c>
-      <c r="F4" s="70" t="s">
-        <v>600</v>
-      </c>
-      <c r="G4" s="70" t="s">
-        <v>600</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>805</v>
-      </c>
-      <c r="I4" s="1">
-        <v>0</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>806</v>
-      </c>
-      <c r="K4" s="22" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:88" x14ac:dyDescent="0.2">
-      <c r="A5" s="82" t="s">
-        <v>201</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>804</v>
-      </c>
-      <c r="F5" s="70" t="s">
-        <v>608</v>
-      </c>
-      <c r="G5" s="70" t="s">
-        <v>608</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>805</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>806</v>
-      </c>
-      <c r="K5" s="22" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -9317,14 +9878,359 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:CJ5"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="32.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" style="1" customWidth="1"/>
+    <col min="6" max="7" width="22.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="26.140625" style="1" customWidth="1"/>
+    <col min="11" max="35" width="22.28515625" style="1" customWidth="1"/>
+    <col min="36" max="36" width="28.85546875" style="1" customWidth="1"/>
+    <col min="37" max="37" width="14.28515625" style="1" customWidth="1"/>
+    <col min="38" max="38" width="23" style="1" customWidth="1"/>
+    <col min="39" max="42" width="19.85546875" style="1" customWidth="1"/>
+    <col min="43" max="44" width="24.7109375" style="1" customWidth="1"/>
+    <col min="45" max="45" width="25" style="1" customWidth="1"/>
+    <col min="46" max="46" width="24.42578125" style="1" customWidth="1"/>
+    <col min="47" max="47" width="30.42578125" style="1" customWidth="1"/>
+    <col min="48" max="48" width="36" style="1" customWidth="1"/>
+    <col min="49" max="49" width="34.42578125" style="1" customWidth="1"/>
+    <col min="50" max="50" width="26.7109375" style="1" customWidth="1"/>
+    <col min="51" max="52" width="17.28515625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="34.140625" style="1" customWidth="1"/>
+    <col min="54" max="54" width="28.42578125" style="1" customWidth="1"/>
+    <col min="55" max="55" width="24.7109375" style="1" customWidth="1"/>
+    <col min="56" max="56" width="30.28515625" style="1" customWidth="1"/>
+    <col min="57" max="57" width="17.5703125" style="1" customWidth="1"/>
+    <col min="58" max="58" width="20.28515625" style="1" customWidth="1"/>
+    <col min="59" max="59" width="12.140625" style="1" customWidth="1"/>
+    <col min="60" max="60" width="21.42578125" style="1" customWidth="1"/>
+    <col min="61" max="61" width="24.140625" style="1" customWidth="1"/>
+    <col min="62" max="62" width="16" style="1" customWidth="1"/>
+    <col min="63" max="63" width="14" style="1" customWidth="1"/>
+    <col min="64" max="64" width="16.7109375" style="1" customWidth="1"/>
+    <col min="65" max="65" width="10.42578125" style="1" customWidth="1"/>
+    <col min="66" max="66" width="37.7109375" style="1" customWidth="1"/>
+    <col min="67" max="68" width="16.7109375" style="1" customWidth="1"/>
+    <col min="69" max="71" width="20.140625" style="1" customWidth="1"/>
+    <col min="72" max="72" width="17.7109375" style="1" customWidth="1"/>
+    <col min="73" max="73" width="24.5703125" style="1" customWidth="1"/>
+    <col min="74" max="76" width="19.42578125" style="1" customWidth="1"/>
+    <col min="77" max="77" width="21.140625" style="1" customWidth="1"/>
+    <col min="78" max="78" width="32.42578125" style="1" customWidth="1"/>
+    <col min="79" max="80" width="17.28515625" style="1" customWidth="1"/>
+    <col min="81" max="83" width="17.5703125" style="1" customWidth="1"/>
+    <col min="84" max="84" width="26.28515625" style="1" customWidth="1"/>
+    <col min="85" max="85" width="35" style="1" customWidth="1"/>
+    <col min="86" max="86" width="26.5703125" style="1" customWidth="1"/>
+    <col min="87" max="87" width="24.85546875" style="1" customWidth="1"/>
+    <col min="88" max="88" width="20" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:88" s="19" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>799</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>616</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>800</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>801</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>802</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>803</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="3"/>
+      <c r="AC1" s="3"/>
+      <c r="AD1" s="3"/>
+      <c r="AE1" s="3"/>
+      <c r="AF1" s="3"/>
+      <c r="AG1" s="3"/>
+      <c r="AH1" s="3"/>
+      <c r="AI1" s="3"/>
+      <c r="AJ1" s="3"/>
+      <c r="AK1" s="3"/>
+      <c r="AL1" s="3"/>
+      <c r="AM1" s="3"/>
+      <c r="AN1" s="3"/>
+      <c r="AO1" s="3"/>
+      <c r="AP1" s="3"/>
+      <c r="AQ1" s="3"/>
+      <c r="AR1" s="3"/>
+      <c r="AS1" s="3"/>
+      <c r="AT1" s="3"/>
+      <c r="AU1" s="3"/>
+      <c r="AV1" s="3"/>
+      <c r="AW1" s="3"/>
+      <c r="AX1" s="3"/>
+      <c r="AY1" s="3"/>
+      <c r="AZ1" s="3"/>
+      <c r="BA1" s="3"/>
+      <c r="BB1" s="3"/>
+      <c r="BC1" s="3"/>
+      <c r="BD1" s="3"/>
+      <c r="BE1" s="3"/>
+      <c r="BF1" s="3"/>
+      <c r="BG1" s="3"/>
+      <c r="BH1" s="3"/>
+      <c r="BI1" s="3"/>
+      <c r="BJ1" s="3"/>
+      <c r="BK1" s="3"/>
+      <c r="BL1" s="3"/>
+      <c r="BM1" s="3"/>
+      <c r="BN1" s="3"/>
+      <c r="BO1" s="3"/>
+      <c r="BP1" s="3"/>
+      <c r="BQ1" s="3"/>
+      <c r="BR1" s="3"/>
+      <c r="BS1" s="3"/>
+      <c r="BT1" s="3"/>
+      <c r="BU1" s="3"/>
+      <c r="BV1" s="3"/>
+      <c r="BW1" s="3"/>
+      <c r="BX1" s="3"/>
+      <c r="BY1" s="3"/>
+      <c r="BZ1" s="3"/>
+      <c r="CA1" s="3"/>
+      <c r="CB1" s="3"/>
+      <c r="CC1" s="3"/>
+      <c r="CD1" s="3"/>
+      <c r="CE1" s="3"/>
+      <c r="CF1" s="3"/>
+      <c r="CG1" s="3"/>
+      <c r="CH1" s="3"/>
+      <c r="CI1" s="3"/>
+      <c r="CJ1" s="3"/>
+    </row>
+    <row r="2" spans="1:88" x14ac:dyDescent="0.2">
+      <c r="A2" s="82" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>773</v>
+      </c>
+      <c r="E2" t="s">
+        <v>804</v>
+      </c>
+      <c r="F2" s="70" t="s">
+        <v>591</v>
+      </c>
+      <c r="G2" s="70" t="s">
+        <v>591</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>806</v>
+      </c>
+      <c r="K2" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="22"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="11"/>
+      <c r="V2" s="11"/>
+      <c r="W2" s="24"/>
+      <c r="X2" s="24"/>
+      <c r="Y2" s="24"/>
+      <c r="Z2" s="25"/>
+      <c r="AA2" s="25"/>
+      <c r="AB2" s="24"/>
+      <c r="AC2" s="24"/>
+      <c r="AD2" s="24"/>
+      <c r="AE2" s="11"/>
+      <c r="AF2" s="11"/>
+    </row>
+    <row r="3" spans="1:88" x14ac:dyDescent="0.2">
+      <c r="A3" s="82" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="F3" s="70" t="s">
+        <v>600</v>
+      </c>
+      <c r="G3" s="70" t="s">
+        <v>600</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>806</v>
+      </c>
+      <c r="K3" s="22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:88" x14ac:dyDescent="0.2">
+      <c r="A4" s="82" t="s">
+        <v>198</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>780</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="F4" s="70" t="s">
+        <v>600</v>
+      </c>
+      <c r="G4" s="70" t="s">
+        <v>606</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>806</v>
+      </c>
+      <c r="K4" s="22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:88" x14ac:dyDescent="0.2">
+      <c r="A5" s="82" t="s">
+        <v>201</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="F5" s="70" t="s">
+        <v>608</v>
+      </c>
+      <c r="G5" s="70" t="s">
+        <v>608</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>806</v>
+      </c>
+      <c r="K5" s="22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
+  <pageSetup paperSize="9" pageOrder="overThenDown" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9636,7 +10542,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -10456,6 +11362,318 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{940E2D94-64DF-4F97-AE3C-B3EE91A208CF}">
+  <dimension ref="A1:AP2"/>
+  <sheetViews>
+    <sheetView topLeftCell="AF1" workbookViewId="0">
+      <selection activeCell="AO2" sqref="AO2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="39.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="27.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="27.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="54.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" style="1" customWidth="1"/>
+    <col min="12" max="13" width="20.7109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="18.85546875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="18" style="1" customWidth="1"/>
+    <col min="18" max="18" width="54" style="1" customWidth="1"/>
+    <col min="19" max="19" width="32.42578125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="54" style="1" customWidth="1"/>
+    <col min="21" max="21" width="39" style="1" customWidth="1"/>
+    <col min="22" max="22" width="24.28515625" style="1" customWidth="1"/>
+    <col min="23" max="23" width="21.5703125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="47" style="1" customWidth="1"/>
+    <col min="25" max="25" width="14.5703125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="14.140625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="32.140625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="21.5703125" style="1" customWidth="1"/>
+    <col min="29" max="29" width="15.85546875" style="1" customWidth="1"/>
+    <col min="30" max="30" width="15.28515625" style="1" customWidth="1"/>
+    <col min="31" max="31" width="54" style="1" customWidth="1"/>
+    <col min="32" max="32" width="28.42578125" style="1" customWidth="1"/>
+    <col min="33" max="33" width="26.28515625" style="1" customWidth="1"/>
+    <col min="34" max="34" width="28.28515625" style="1" customWidth="1"/>
+    <col min="35" max="35" width="16.42578125" style="1" customWidth="1"/>
+    <col min="36" max="36" width="21.42578125" style="1" customWidth="1"/>
+    <col min="37" max="37" width="17.85546875" style="1" customWidth="1"/>
+    <col min="38" max="39" width="21" style="1" customWidth="1"/>
+    <col min="40" max="40" width="22" style="1" customWidth="1"/>
+    <col min="41" max="41" width="20.140625" style="1" customWidth="1"/>
+    <col min="42" max="42" width="23.42578125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:42" s="94" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="92" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="92" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="93" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="93" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="92" t="s">
+        <v>874</v>
+      </c>
+      <c r="F1" s="92" t="s">
+        <v>875</v>
+      </c>
+      <c r="G1" s="92" t="s">
+        <v>876</v>
+      </c>
+      <c r="H1" s="93" t="s">
+        <v>877</v>
+      </c>
+      <c r="I1" s="92" t="s">
+        <v>878</v>
+      </c>
+      <c r="J1" s="92" t="s">
+        <v>879</v>
+      </c>
+      <c r="K1" s="92" t="s">
+        <v>880</v>
+      </c>
+      <c r="L1" s="92" t="s">
+        <v>881</v>
+      </c>
+      <c r="M1" s="92" t="s">
+        <v>882</v>
+      </c>
+      <c r="N1" s="92" t="s">
+        <v>883</v>
+      </c>
+      <c r="O1" s="92" t="s">
+        <v>884</v>
+      </c>
+      <c r="P1" s="92" t="s">
+        <v>885</v>
+      </c>
+      <c r="Q1" s="92" t="s">
+        <v>886</v>
+      </c>
+      <c r="R1" s="92" t="s">
+        <v>887</v>
+      </c>
+      <c r="S1" s="92" t="s">
+        <v>888</v>
+      </c>
+      <c r="T1" s="92" t="s">
+        <v>889</v>
+      </c>
+      <c r="U1" s="92" t="s">
+        <v>890</v>
+      </c>
+      <c r="V1" s="92" t="s">
+        <v>891</v>
+      </c>
+      <c r="W1" s="92" t="s">
+        <v>892</v>
+      </c>
+      <c r="X1" s="92" t="s">
+        <v>893</v>
+      </c>
+      <c r="Y1" s="92" t="s">
+        <v>894</v>
+      </c>
+      <c r="Z1" s="92" t="s">
+        <v>895</v>
+      </c>
+      <c r="AA1" s="92" t="s">
+        <v>896</v>
+      </c>
+      <c r="AB1" s="92" t="s">
+        <v>897</v>
+      </c>
+      <c r="AC1" s="92" t="s">
+        <v>898</v>
+      </c>
+      <c r="AD1" s="92" t="s">
+        <v>899</v>
+      </c>
+      <c r="AE1" s="92" t="s">
+        <v>900</v>
+      </c>
+      <c r="AF1" s="92" t="s">
+        <v>901</v>
+      </c>
+      <c r="AG1" s="92" t="s">
+        <v>902</v>
+      </c>
+      <c r="AH1" s="92" t="s">
+        <v>903</v>
+      </c>
+      <c r="AI1" s="8" t="s">
+        <v>904</v>
+      </c>
+      <c r="AJ1" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="AK1" s="8" t="s">
+        <v>905</v>
+      </c>
+      <c r="AL1" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="AM1" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="AN1" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="AO1" s="8" t="s">
+        <v>906</v>
+      </c>
+      <c r="AP1" s="8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:42" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>907</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>780</v>
+      </c>
+      <c r="E2" s="95" t="s">
+        <v>908</v>
+      </c>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95" t="s">
+        <v>909</v>
+      </c>
+      <c r="H2" s="75" t="s">
+        <v>806</v>
+      </c>
+      <c r="I2" s="60" t="s">
+        <v>925</v>
+      </c>
+      <c r="J2" s="95" t="s">
+        <v>179</v>
+      </c>
+      <c r="K2" s="95" t="s">
+        <v>182</v>
+      </c>
+      <c r="L2" s="95" t="s">
+        <v>185</v>
+      </c>
+      <c r="M2" s="95" t="s">
+        <v>186</v>
+      </c>
+      <c r="N2" s="97" t="s">
+        <v>927</v>
+      </c>
+      <c r="O2" s="96" t="s">
+        <v>184</v>
+      </c>
+      <c r="P2" s="98" t="s">
+        <v>928</v>
+      </c>
+      <c r="Q2" s="95" t="s">
+        <v>911</v>
+      </c>
+      <c r="R2" s="95" t="s">
+        <v>912</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>910</v>
+      </c>
+      <c r="T2" s="95" t="s">
+        <v>929</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>910</v>
+      </c>
+      <c r="V2" s="95" t="s">
+        <v>913</v>
+      </c>
+      <c r="W2" s="95" t="s">
+        <v>914</v>
+      </c>
+      <c r="X2" s="95" t="s">
+        <v>915</v>
+      </c>
+      <c r="Y2" s="95" t="s">
+        <v>916</v>
+      </c>
+      <c r="Z2" s="95" t="s">
+        <v>917</v>
+      </c>
+      <c r="AA2" s="95" t="s">
+        <v>918</v>
+      </c>
+      <c r="AB2" s="95" t="s">
+        <v>919</v>
+      </c>
+      <c r="AC2" s="95" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD2" s="95" t="s">
+        <v>920</v>
+      </c>
+      <c r="AE2" s="95" t="s">
+        <v>921</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>922</v>
+      </c>
+      <c r="AG2" s="95" t="s">
+        <v>923</v>
+      </c>
+      <c r="AH2" s="95" t="s">
+        <v>179</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="AJ2" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="AL2" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="AM2" s="11" t="s">
+        <v>924</v>
+      </c>
+      <c r="AN2" s="1">
+        <v>6</v>
+      </c>
+      <c r="AO2" s="75" t="s">
+        <v>926</v>
+      </c>
+      <c r="AP2" s="75" t="s">
+        <v>537</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -10649,7 +11867,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -10949,7 +12167,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -11141,7 +12359,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -12296,7 +13514,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -12963,714 +14181,4 @@
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
   <pageSetup paperSize="9" pageOrder="overThenDown" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:AQ5"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="6.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17" style="1" customWidth="1"/>
-    <col min="8" max="8" width="24.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="23.140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="18.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="20.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="23.140625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="31.28515625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="18" style="1" customWidth="1"/>
-    <col min="17" max="17" width="21.5703125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="21.7109375" style="1" customWidth="1"/>
-    <col min="19" max="19" width="26.5703125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="19.42578125" style="1" customWidth="1"/>
-    <col min="21" max="21" width="32.7109375" style="1" customWidth="1"/>
-    <col min="22" max="22" width="21" style="1" customWidth="1"/>
-    <col min="23" max="23" width="18.28515625" style="1" customWidth="1"/>
-    <col min="24" max="24" width="20" style="1" customWidth="1"/>
-    <col min="25" max="26" width="19.85546875" style="1" customWidth="1"/>
-    <col min="27" max="28" width="25.85546875" style="1" customWidth="1"/>
-    <col min="29" max="30" width="26.5703125" style="1" customWidth="1"/>
-    <col min="31" max="32" width="25.5703125" style="1" customWidth="1"/>
-    <col min="33" max="34" width="26.85546875" style="1" customWidth="1"/>
-    <col min="35" max="37" width="14.85546875" style="1" customWidth="1"/>
-    <col min="38" max="39" width="20.42578125" style="1" customWidth="1"/>
-    <col min="40" max="41" width="33" style="1" customWidth="1"/>
-    <col min="42" max="43" width="16.85546875" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:43" s="28" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>550</v>
-      </c>
-      <c r="D1" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="28" t="s">
-        <v>460</v>
-      </c>
-      <c r="G1" s="28" t="s">
-        <v>551</v>
-      </c>
-      <c r="H1" s="28" t="s">
-        <v>552</v>
-      </c>
-      <c r="I1" s="28" t="s">
-        <v>553</v>
-      </c>
-      <c r="J1" s="28" t="s">
-        <v>554</v>
-      </c>
-      <c r="K1" s="28" t="s">
-        <v>555</v>
-      </c>
-      <c r="L1" s="28" t="s">
-        <v>556</v>
-      </c>
-      <c r="M1" s="28" t="s">
-        <v>557</v>
-      </c>
-      <c r="N1" s="28" t="s">
-        <v>558</v>
-      </c>
-      <c r="O1" s="28" t="s">
-        <v>559</v>
-      </c>
-      <c r="P1" s="28" t="s">
-        <v>560</v>
-      </c>
-      <c r="Q1" s="28" t="s">
-        <v>561</v>
-      </c>
-      <c r="R1" s="28" t="s">
-        <v>562</v>
-      </c>
-      <c r="S1" s="28" t="s">
-        <v>563</v>
-      </c>
-      <c r="T1" s="28" t="s">
-        <v>564</v>
-      </c>
-      <c r="U1" s="28" t="s">
-        <v>565</v>
-      </c>
-      <c r="V1" s="28" t="s">
-        <v>566</v>
-      </c>
-      <c r="W1" s="28" t="s">
-        <v>567</v>
-      </c>
-      <c r="X1" s="28" t="s">
-        <v>568</v>
-      </c>
-      <c r="Y1" s="28" t="s">
-        <v>569</v>
-      </c>
-      <c r="Z1" s="28" t="s">
-        <v>570</v>
-      </c>
-      <c r="AA1" s="28" t="s">
-        <v>571</v>
-      </c>
-      <c r="AB1" s="28" t="s">
-        <v>572</v>
-      </c>
-      <c r="AC1" s="28" t="s">
-        <v>573</v>
-      </c>
-      <c r="AD1" s="28" t="s">
-        <v>574</v>
-      </c>
-      <c r="AE1" s="28" t="s">
-        <v>575</v>
-      </c>
-      <c r="AF1" s="28" t="s">
-        <v>576</v>
-      </c>
-      <c r="AG1" s="28" t="s">
-        <v>577</v>
-      </c>
-      <c r="AH1" s="28" t="s">
-        <v>578</v>
-      </c>
-      <c r="AI1" s="28" t="s">
-        <v>579</v>
-      </c>
-      <c r="AJ1" s="28" t="s">
-        <v>580</v>
-      </c>
-      <c r="AK1" s="28" t="s">
-        <v>581</v>
-      </c>
-      <c r="AL1" s="28" t="s">
-        <v>582</v>
-      </c>
-      <c r="AM1" s="28" t="s">
-        <v>583</v>
-      </c>
-      <c r="AN1" s="28" t="s">
-        <v>584</v>
-      </c>
-      <c r="AO1" s="28" t="s">
-        <v>585</v>
-      </c>
-      <c r="AP1" s="28" t="s">
-        <v>586</v>
-      </c>
-      <c r="AQ1" s="28" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="2" spans="1:43" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>588</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>589</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>260</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>590</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>591</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="P2" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>592</v>
-      </c>
-      <c r="R2" s="12" t="s">
-        <v>593</v>
-      </c>
-      <c r="S2" s="9" t="s">
-        <v>594</v>
-      </c>
-      <c r="T2" s="9" t="s">
-        <v>593</v>
-      </c>
-      <c r="U2" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="V2" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="X2" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="Y2" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z2" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="AA2" s="9" t="s">
-        <v>593</v>
-      </c>
-      <c r="AB2" s="9" t="s">
-        <v>593</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>595</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>595</v>
-      </c>
-      <c r="AE2" s="9" t="s">
-        <v>596</v>
-      </c>
-      <c r="AF2" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="AG2" s="9" t="s">
-        <v>597</v>
-      </c>
-      <c r="AH2" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="AI2" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ2" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="AK2" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="AL2" s="9" t="s">
-        <v>593</v>
-      </c>
-      <c r="AM2" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="AN2" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="AO2" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="AP2" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="AQ2" s="9" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="3" spans="1:43" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>598</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>599</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>261</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="L3" s="9" t="s">
-        <v>591</v>
-      </c>
-      <c r="M3" s="9" t="s">
-        <v>600</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="O3" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="P3" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q3" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="R3" s="12" t="s">
-        <v>593</v>
-      </c>
-      <c r="S3" s="9" t="s">
-        <v>594</v>
-      </c>
-      <c r="T3" s="9" t="s">
-        <v>593</v>
-      </c>
-      <c r="U3" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="V3" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="X3" s="9" t="s">
-        <v>601</v>
-      </c>
-      <c r="Y3" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z3" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="AA3" s="9" t="s">
-        <v>593</v>
-      </c>
-      <c r="AB3" s="9" t="s">
-        <v>593</v>
-      </c>
-      <c r="AC3" s="1" t="s">
-        <v>595</v>
-      </c>
-      <c r="AD3" s="1" t="s">
-        <v>595</v>
-      </c>
-      <c r="AE3" s="9" t="s">
-        <v>596</v>
-      </c>
-      <c r="AF3" s="9" t="s">
-        <v>596</v>
-      </c>
-      <c r="AG3" s="9" t="s">
-        <v>602</v>
-      </c>
-      <c r="AH3" s="9" t="s">
-        <v>597</v>
-      </c>
-      <c r="AI3" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ3" s="9" t="s">
-        <v>414</v>
-      </c>
-      <c r="AK3" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="AL3" s="9" t="s">
-        <v>593</v>
-      </c>
-      <c r="AM3" s="9" t="s">
-        <v>593</v>
-      </c>
-      <c r="AN3" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="AO3" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="AP3" s="9" t="s">
-        <v>526</v>
-      </c>
-      <c r="AQ3" s="9" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="4" spans="1:43" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>603</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>599</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>262</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>604</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>605</v>
-      </c>
-      <c r="M4" s="9" t="s">
-        <v>606</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="O4" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="P4" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q4" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="R4" s="12" t="s">
-        <v>593</v>
-      </c>
-      <c r="S4" s="9" t="s">
-        <v>594</v>
-      </c>
-      <c r="T4" s="9" t="s">
-        <v>593</v>
-      </c>
-      <c r="U4" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="V4" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="X4" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="Y4" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z4" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="AA4" s="9" t="s">
-        <v>593</v>
-      </c>
-      <c r="AB4" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="AC4" s="1" t="s">
-        <v>595</v>
-      </c>
-      <c r="AD4" s="1" t="s">
-        <v>595</v>
-      </c>
-      <c r="AE4" s="9" t="s">
-        <v>596</v>
-      </c>
-      <c r="AF4" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="AG4" s="9" t="s">
-        <v>602</v>
-      </c>
-      <c r="AH4" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="AI4" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ4" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="AK4" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="AL4" s="9" t="s">
-        <v>593</v>
-      </c>
-      <c r="AM4" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="AN4" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="AO4" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="AP4" s="9" t="s">
-        <v>526</v>
-      </c>
-      <c r="AQ4" s="9" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="5" spans="1:43" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>607</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>599</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>263</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>604</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="L5" s="9" t="s">
-        <v>600</v>
-      </c>
-      <c r="M5" s="9" t="s">
-        <v>608</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="O5" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="P5" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q5" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="R5" s="12" t="s">
-        <v>593</v>
-      </c>
-      <c r="S5" s="9" t="s">
-        <v>594</v>
-      </c>
-      <c r="T5" s="9" t="s">
-        <v>593</v>
-      </c>
-      <c r="U5" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="V5" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="X5" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="Y5" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z5" s="9" t="s">
-        <v>414</v>
-      </c>
-      <c r="AA5" s="9" t="s">
-        <v>593</v>
-      </c>
-      <c r="AB5" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="AC5" s="1" t="s">
-        <v>595</v>
-      </c>
-      <c r="AD5" s="1" t="s">
-        <v>595</v>
-      </c>
-      <c r="AE5" s="9" t="s">
-        <v>596</v>
-      </c>
-      <c r="AF5" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="AG5" s="9" t="s">
-        <v>602</v>
-      </c>
-      <c r="AH5" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="AI5" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ5" s="9" t="s">
-        <v>414</v>
-      </c>
-      <c r="AK5" s="9" t="s">
-        <v>426</v>
-      </c>
-      <c r="AL5" s="9" t="s">
-        <v>593</v>
-      </c>
-      <c r="AM5" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="AN5" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="AO5" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="AP5" s="9" t="s">
-        <v>526</v>
-      </c>
-      <c r="AQ5" s="9" t="s">
-        <v>375</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
-  <pageSetup paperSize="9" pageOrder="overThenDown" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
 </file>
</xml_diff>